<commit_message>
More inventory tests: Add and remove
</commit_message>
<xml_diff>
--- a/webtesting/dataProviders/Inventory.xlsx
+++ b/webtesting/dataProviders/Inventory.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelrodriguez/repo/webtesting_challenge/webtesting/dataProviders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42BDEA8-CBB0-0C4B-87C7-ABFB33F98EED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF147FB2-13B6-7746-B877-72BD4E7D6141}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32840" yWindow="460" windowWidth="32840" windowHeight="20540" activeTab="1" xr2:uid="{44DC75CC-9B3D-4B43-A129-81E7F5B5599D}"/>
+    <workbookView xWindow="-32840" yWindow="2680" windowWidth="32840" windowHeight="20540" activeTab="2" xr2:uid="{44DC75CC-9B3D-4B43-A129-81E7F5B5599D}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
     <sheet name="Sort" sheetId="2" r:id="rId2"/>
+    <sheet name="ID" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -503,7 +504,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection sqref="A1:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -651,7 +652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDBDF6A-CF0D-344E-AA7E-762C1E56733A}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -685,4 +686,54 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2366F193-5011-AA49-BE21-1A295C44FC01}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finished remove from cart tests
</commit_message>
<xml_diff>
--- a/webtesting/dataProviders/Inventory.xlsx
+++ b/webtesting/dataProviders/Inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelrodriguez/repo/webtesting_challenge/webtesting/dataProviders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF147FB2-13B6-7746-B877-72BD4E7D6141}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5199B72-223A-9045-B06F-8F92CFE9B9AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32840" yWindow="2680" windowWidth="32840" windowHeight="20540" activeTab="2" xr2:uid="{44DC75CC-9B3D-4B43-A129-81E7F5B5599D}"/>
   </bookViews>
@@ -693,7 +693,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Started product page tests
</commit_message>
<xml_diff>
--- a/webtesting/dataProviders/Inventory.xlsx
+++ b/webtesting/dataProviders/Inventory.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelrodriguez/repo/webtesting_challenge/webtesting/dataProviders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5199B72-223A-9045-B06F-8F92CFE9B9AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1552D9FB-D70A-7E48-89BA-771498FB55E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32840" yWindow="2680" windowWidth="32840" windowHeight="20540" activeTab="2" xr2:uid="{44DC75CC-9B3D-4B43-A129-81E7F5B5599D}"/>
+    <workbookView xWindow="-32840" yWindow="2680" windowWidth="32840" windowHeight="20540" activeTab="3" xr2:uid="{44DC75CC-9B3D-4B43-A129-81E7F5B5599D}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
     <sheet name="Sort" sheetId="2" r:id="rId2"/>
     <sheet name="ID" sheetId="3" r:id="rId3"/>
+    <sheet name="Products" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -504,7 +505,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A7"/>
+      <selection activeCell="B7" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -692,7 +693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2366F193-5011-AA49-BE21-1A295C44FC01}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -736,4 +737,153 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B2822B0-F32A-1148-B787-2876F641DCA3}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="57.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="70.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{1B646214-45AD-DE4E-AB96-113EDE20B05D}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{BE5CA31C-1E22-5E46-A87E-00D18A502B5F}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{44D1057C-DD36-264D-B8DC-B70DA47ED5A6}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{E655E439-03ED-AC4B-B1B5-C97AF3213E0B}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{9184F4E6-8CD7-4840-8DEE-7942EDBA63D9}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{91554816-1892-AA4E-A6F1-2B6849241DBB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Created Excel file with data provider
</commit_message>
<xml_diff>
--- a/webtesting/dataProviders/Inventory.xlsx
+++ b/webtesting/dataProviders/Inventory.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelrodriguez/repo/webtesting_challenge/webtesting/dataProviders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1552D9FB-D70A-7E48-89BA-771498FB55E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A88DE2A-8063-C142-8305-13BA95D6731A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32840" yWindow="2680" windowWidth="32840" windowHeight="20540" activeTab="3" xr2:uid="{44DC75CC-9B3D-4B43-A129-81E7F5B5599D}"/>
+    <workbookView xWindow="-32800" yWindow="460" windowWidth="32800" windowHeight="20540" activeTab="4" xr2:uid="{44DC75CC-9B3D-4B43-A129-81E7F5B5599D}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
     <sheet name="Sort" sheetId="2" r:id="rId2"/>
     <sheet name="ID" sheetId="3" r:id="rId3"/>
     <sheet name="Products" sheetId="4" r:id="rId4"/>
+    <sheet name="Cart" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="40">
   <si>
     <t>ID</t>
   </si>
@@ -135,6 +136,27 @@
   </si>
   <si>
     <t>hilo</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/inventory-item.html?id=4</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/inventory-item.html?id=0</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/inventory-item.html?id=1</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/inventory-item.html?id=5</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/inventory-item.html?id=2</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/inventory-item.html?id=3</t>
   </si>
 </sst>
 </file>
@@ -505,7 +527,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B2:B7"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -694,7 +716,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -743,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B2822B0-F32A-1148-B787-2876F641DCA3}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -886,4 +908,153 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD455EA-35AD-D84E-A6F2-53EE79D7BC6E}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="48.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{CEB2FC3F-6857-134B-9F8C-22D62949B1BE}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{29D75FDE-79AA-F14A-8BCD-D72AF1E16D1F}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{E8FB1AFF-2428-CF4A-BADE-824641DC2A78}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{B4692E63-0275-9943-8F82-B4A883144DE9}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{17884B61-4850-264D-95A9-5970D7F10321}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{AAD72FB9-A9E5-E245-9B11-E5D3F4AF3E94}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added a test for every shopping cart element in UI
</commit_message>
<xml_diff>
--- a/webtesting/dataProviders/Inventory.xlsx
+++ b/webtesting/dataProviders/Inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelrodriguez/repo/webtesting_challenge/webtesting/dataProviders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A88DE2A-8063-C142-8305-13BA95D6731A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E66F5A-9202-E14C-9066-5E08FF0EE99B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32800" yWindow="460" windowWidth="32800" windowHeight="20540" activeTab="4" xr2:uid="{44DC75CC-9B3D-4B43-A129-81E7F5B5599D}"/>
+    <workbookView xWindow="-32740" yWindow="460" windowWidth="32740" windowHeight="20540" activeTab="4" xr2:uid="{44DC75CC-9B3D-4B43-A129-81E7F5B5599D}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
   <si>
     <t>ID</t>
   </si>
@@ -915,7 +915,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -957,8 +957,8 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
+      <c r="E2" s="1">
+        <v>29.99</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="68" x14ac:dyDescent="0.2">
@@ -974,8 +974,8 @@
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
+      <c r="E3" s="1">
+        <v>9.99</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="68" x14ac:dyDescent="0.2">
@@ -991,8 +991,8 @@
       <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
+      <c r="E4" s="1">
+        <v>15.99</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="68" x14ac:dyDescent="0.2">
@@ -1008,8 +1008,8 @@
       <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>20</v>
+      <c r="E5" s="1">
+        <v>49.99</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="68" x14ac:dyDescent="0.2">
@@ -1025,8 +1025,8 @@
       <c r="D6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>24</v>
+      <c r="E6" s="1">
+        <v>7.99</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="68" x14ac:dyDescent="0.2">
@@ -1042,8 +1042,8 @@
       <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>16</v>
+      <c r="E7" s="1">
+        <v>15.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arranged some code and also TestNG XML files
</commit_message>
<xml_diff>
--- a/webtesting/dataProviders/Inventory.xlsx
+++ b/webtesting/dataProviders/Inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelrodriguez/repo/webtesting_challenge/webtesting/dataProviders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E66F5A-9202-E14C-9066-5E08FF0EE99B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91BE871-F81D-504F-8AF0-802849649AE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32740" yWindow="460" windowWidth="32740" windowHeight="20540" activeTab="4" xr2:uid="{44DC75CC-9B3D-4B43-A129-81E7F5B5599D}"/>
+    <workbookView xWindow="-32700" yWindow="460" windowWidth="32700" windowHeight="20540" xr2:uid="{44DC75CC-9B3D-4B43-A129-81E7F5B5599D}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA95EFF8-74AF-8043-9439-75C121A28058}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -914,7 +914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD455EA-35AD-D84E-A6F2-53EE79D7BC6E}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Refactored Ui check for product page, using soft asserts
</commit_message>
<xml_diff>
--- a/webtesting/dataProviders/Inventory.xlsx
+++ b/webtesting/dataProviders/Inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelrodriguez/repo/webtesting_challenge/webtesting/dataProviders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91BE871-F81D-504F-8AF0-802849649AE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2A826F-71A5-D345-A213-671F83710787}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32700" yWindow="460" windowWidth="32700" windowHeight="20540" xr2:uid="{44DC75CC-9B3D-4B43-A129-81E7F5B5599D}"/>
+    <workbookView xWindow="-32700" yWindow="460" windowWidth="32700" windowHeight="20540" activeTab="3" xr2:uid="{44DC75CC-9B3D-4B43-A129-81E7F5B5599D}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -157,6 +157,24 @@
   </si>
   <si>
     <t>https://www.saucedemo.com/inventory-item.html?id=3</t>
+  </si>
+  <si>
+    <t>sauce-backpack-1200x1500</t>
+  </si>
+  <si>
+    <t>bike-light-1200x1500</t>
+  </si>
+  <si>
+    <t>bolt-shirt-1200x1500</t>
+  </si>
+  <si>
+    <t>sauce-pullover-1200x1500</t>
+  </si>
+  <si>
+    <t>red-onesie-1200x1500</t>
+  </si>
+  <si>
+    <t>red-tatt-1200x1500</t>
   </si>
 </sst>
 </file>
@@ -201,7 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -209,6 +227,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -526,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA95EFF8-74AF-8043-9439-75C121A28058}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -765,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B2822B0-F32A-1148-B787-2876F641DCA3}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -799,8 +818,8 @@
       <c r="A2" s="1">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="B2" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -816,8 +835,8 @@
       <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
+      <c r="B3" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -833,8 +852,8 @@
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
+      <c r="B4" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
@@ -850,8 +869,8 @@
       <c r="A5" s="1">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
+      <c r="B5" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>18</v>
@@ -867,8 +886,8 @@
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
+      <c r="B6" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>22</v>
@@ -884,8 +903,8 @@
       <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>25</v>
+      <c r="B7" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>26</v>
@@ -898,14 +917,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{1B646214-45AD-DE4E-AB96-113EDE20B05D}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{BE5CA31C-1E22-5E46-A87E-00D18A502B5F}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{44D1057C-DD36-264D-B8DC-B70DA47ED5A6}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{E655E439-03ED-AC4B-B1B5-C97AF3213E0B}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{9184F4E6-8CD7-4840-8DEE-7942EDBA63D9}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{91554816-1892-AA4E-A6F1-2B6849241DBB}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Refactored UI validations on Inventory Page, and applied soft asserts on inventory tests
</commit_message>
<xml_diff>
--- a/webtesting/dataProviders/Inventory.xlsx
+++ b/webtesting/dataProviders/Inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelrodriguez/repo/webtesting_challenge/webtesting/dataProviders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2A826F-71A5-D345-A213-671F83710787}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51B4770-0B1D-354E-8F64-AEBD04A98AB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32700" yWindow="460" windowWidth="32700" windowHeight="20540" activeTab="3" xr2:uid="{44DC75CC-9B3D-4B43-A129-81E7F5B5599D}"/>
+    <workbookView xWindow="-32700" yWindow="460" windowWidth="32700" windowHeight="20540" xr2:uid="{44DC75CC-9B3D-4B43-A129-81E7F5B5599D}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
   <si>
     <t>ID</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Price</t>
   </si>
   <si>
-    <t>https://www.saucedemo.com/img/sauce-backpack-1200x1500.jpg</t>
-  </si>
-  <si>
     <t>Sauce Labs Backpack</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>$29.99</t>
   </si>
   <si>
-    <t>https://www.saucedemo.com/img/bike-light-1200x1500.jpg</t>
-  </si>
-  <si>
     <t>Sauce Labs Bike Light</t>
   </si>
   <si>
@@ -78,9 +72,6 @@
     <t>$9.99</t>
   </si>
   <si>
-    <t>https://www.saucedemo.com/img/bolt-shirt-1200x1500.jpg</t>
-  </si>
-  <si>
     <t>Sauce Labs Bolt T-Shirt</t>
   </si>
   <si>
@@ -90,9 +81,6 @@
     <t>$15.99</t>
   </si>
   <si>
-    <t>https://www.saucedemo.com/img/sauce-pullover-1200x1500.jpg</t>
-  </si>
-  <si>
     <t>Sauce Labs Fleece Jacket</t>
   </si>
   <si>
@@ -102,9 +90,6 @@
     <t>$49.99</t>
   </si>
   <si>
-    <t>https://www.saucedemo.com/img/red-onesie-1200x1500.jpg</t>
-  </si>
-  <si>
     <t>Sauce Labs Onesie</t>
   </si>
   <si>
@@ -112,9 +97,6 @@
   </si>
   <si>
     <t>$7.99</t>
-  </si>
-  <si>
-    <t>https://www.saucedemo.com/img/red-tatt-1200x1500.jpg</t>
   </si>
   <si>
     <t>Test.allTheThings() T-Shirt (Red)</t>
@@ -545,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA95EFF8-74AF-8043-9439-75C121A28058}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -579,113 +561,105 @@
       <c r="A2" s="1">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
+      <c r="B5" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
+      <c r="B6" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>25</v>
+      <c r="B7" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{61E26CB2-334A-CB42-9530-D7DC8B8B7010}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{E9953262-7100-FF43-82B2-0B4F5353D30E}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{434C83DA-7C49-6742-9E1E-048FC30B7701}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{9E76EB6A-8B6A-424E-BE93-3D8DDABE4ECB}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{430CF4C4-AA1F-3F4F-9A1B-C59A0F74D850}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{EC6089F6-05B2-A842-9DA9-4DF2F934325D}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -702,27 +676,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -784,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B2822B0-F32A-1148-B787-2876F641DCA3}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="133" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -819,16 +793,16 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -836,16 +810,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -853,16 +827,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -870,16 +844,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -887,16 +861,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -904,16 +878,16 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -943,7 +917,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -960,13 +934,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="E2" s="1">
         <v>29.99</v>
@@ -977,13 +951,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1">
         <v>9.99</v>
@@ -994,13 +968,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1">
         <v>15.99</v>
@@ -1011,13 +985,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E5" s="1">
         <v>49.99</v>
@@ -1028,13 +1002,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E6" s="1">
         <v>7.99</v>
@@ -1045,13 +1019,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1">
         <v>15.99</v>

</xml_diff>

<commit_message>
Added oft assert for Shopping cart Ui tests, besides some other changes on inventory page
</commit_message>
<xml_diff>
--- a/webtesting/dataProviders/Inventory.xlsx
+++ b/webtesting/dataProviders/Inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelrodriguez/repo/webtesting_challenge/webtesting/dataProviders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51B4770-0B1D-354E-8F64-AEBD04A98AB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE5D6BE-A757-E243-AE99-5D411E8CB915}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32700" yWindow="460" windowWidth="32700" windowHeight="20540" xr2:uid="{44DC75CC-9B3D-4B43-A129-81E7F5B5599D}"/>
+    <workbookView xWindow="-32700" yWindow="460" windowWidth="32700" windowHeight="20540" activeTab="4" xr2:uid="{44DC75CC-9B3D-4B43-A129-81E7F5B5599D}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -118,27 +118,6 @@
   </si>
   <si>
     <t>hilo</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>https://www.saucedemo.com/inventory-item.html?id=4</t>
-  </si>
-  <si>
-    <t>https://www.saucedemo.com/inventory-item.html?id=0</t>
-  </si>
-  <si>
-    <t>https://www.saucedemo.com/inventory-item.html?id=1</t>
-  </si>
-  <si>
-    <t>https://www.saucedemo.com/inventory-item.html?id=5</t>
-  </si>
-  <si>
-    <t>https://www.saucedemo.com/inventory-item.html?id=2</t>
-  </si>
-  <si>
-    <t>https://www.saucedemo.com/inventory-item.html?id=3</t>
   </si>
   <si>
     <t>sauce-backpack-1200x1500</t>
@@ -163,18 +142,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -197,22 +168,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,7 +493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA95EFF8-74AF-8043-9439-75C121A28058}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -561,8 +527,8 @@
       <c r="A2" s="1">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>34</v>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -578,8 +544,8 @@
       <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>35</v>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -595,8 +561,8 @@
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>36</v>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -612,8 +578,8 @@
       <c r="A5" s="1">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>37</v>
+      <c r="B5" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
@@ -629,8 +595,8 @@
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>38</v>
+      <c r="B6" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>17</v>
@@ -646,8 +612,8 @@
       <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>39</v>
+      <c r="B7" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>20</v>
@@ -792,8 +758,8 @@
       <c r="A2" s="1">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>34</v>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -809,8 +775,8 @@
       <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>35</v>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -826,8 +792,8 @@
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>36</v>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -843,8 +809,8 @@
       <c r="A5" s="1">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>37</v>
+      <c r="B5" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
@@ -860,8 +826,8 @@
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>38</v>
+      <c r="B6" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>17</v>
@@ -877,8 +843,8 @@
       <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>39</v>
+      <c r="B7" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>20</v>
@@ -897,149 +863,119 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD455EA-35AD-D84E-A6F2-53EE79D7BC6E}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="48.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="13.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>28</v>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1">
+      <c r="D2" s="1">
         <v>29.99</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>29</v>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1">
+      <c r="D3" s="1">
         <v>9.99</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>30</v>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1">
+      <c r="D4" s="1">
         <v>15.99</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>31</v>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="1">
+      <c r="D5" s="1">
         <v>49.99</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>32</v>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="1">
+      <c r="D6" s="1">
         <v>7.99</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>33</v>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="1">
+      <c r="D7" s="1">
         <v>15.99</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{CEB2FC3F-6857-134B-9F8C-22D62949B1BE}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{29D75FDE-79AA-F14A-8BCD-D72AF1E16D1F}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{E8FB1AFF-2428-CF4A-BADE-824641DC2A78}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{B4692E63-0275-9943-8F82-B4A883144DE9}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{17884B61-4850-264D-95A9-5970D7F10321}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{AAD72FB9-A9E5-E245-9B11-E5D3F4AF3E94}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactored the test to remove individual products, to do it by name
</commit_message>
<xml_diff>
--- a/webtesting/dataProviders/Inventory.xlsx
+++ b/webtesting/dataProviders/Inventory.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelrodriguez/repo/webtesting_challenge/webtesting/dataProviders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE5D6BE-A757-E243-AE99-5D411E8CB915}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF17810-703C-5C4E-B5C4-D7AE473BEBC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32700" yWindow="460" windowWidth="32700" windowHeight="20540" activeTab="4" xr2:uid="{44DC75CC-9B3D-4B43-A129-81E7F5B5599D}"/>
+    <workbookView xWindow="-32700" yWindow="460" windowWidth="32700" windowHeight="20540" activeTab="3" xr2:uid="{44DC75CC-9B3D-4B43-A129-81E7F5B5599D}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
     <sheet name="Sort" sheetId="2" r:id="rId2"/>
     <sheet name="ID" sheetId="3" r:id="rId3"/>
-    <sheet name="Products" sheetId="4" r:id="rId4"/>
-    <sheet name="Cart" sheetId="5" r:id="rId5"/>
+    <sheet name="Names" sheetId="6" r:id="rId4"/>
+    <sheet name="Products" sheetId="4" r:id="rId5"/>
+    <sheet name="Cart" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -142,10 +143,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -171,12 +179,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,7 +505,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C1" sqref="C1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -675,7 +686,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+      <selection sqref="A1:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -721,6 +732,77 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49DEB47B-2BAF-9E42-926A-6A7A8B1A8DAB}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B2822B0-F32A-1148-B787-2876F641DCA3}">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -861,11 +943,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD455EA-35AD-D84E-A6F2-53EE79D7BC6E}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>